<commit_message>
removed extra files that should have been ignored
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">person</t>
   </si>
@@ -38,6 +38,24 @@
   </si>
   <si>
     <t xml:space="preserve">15;15;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unplanned;POM25;POM26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5;25;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin;24BES;24Spend plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15;8;17</t>
   </si>
 </sst>
 </file>
@@ -141,7 +159,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="A3:C4"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="1" sqref="A3:C4 F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -169,14 +187,26 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>

</xml_diff>